<commit_message>
Refactor code to include parallel versions of hill-climbing and simulated-annealing algorithms
</commit_message>
<xml_diff>
--- a/Trabajo/Data/test/12threadsCompleto.xlsx
+++ b/Trabajo/Data/test/12threadsCompleto.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ketbome\Desktop\Projects\Electivo\Trabajo\Data\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5B108E-6031-40F9-8ABD-E0C99B802AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiempos" sheetId="1" r:id="rId1"/>
     <sheet name="Nodos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -144,8 +150,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,7 +212,308 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="44">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -216,13 +523,21 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -260,7 +575,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -294,6 +609,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -328,9 +644,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -503,14 +820,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -536,7 +862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -562,7 +888,7 @@
         <v>1475.97</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -588,7 +914,7 @@
         <v>1500.52</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -614,7 +940,7 @@
         <v>761.46</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -622,7 +948,7 @@
         <v>71.2</v>
       </c>
       <c r="C5">
-        <v>70.59999999999999</v>
+        <v>70.599999999999994</v>
       </c>
       <c r="D5">
         <v>116.5</v>
@@ -631,7 +957,7 @@
         <v>73.98</v>
       </c>
       <c r="F5">
-        <v>76.26000000000001</v>
+        <v>76.260000000000005</v>
       </c>
       <c r="G5">
         <v>72.45</v>
@@ -640,7 +966,7 @@
         <v>74.22</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -654,24 +980,24 @@
         <v>460.42</v>
       </c>
       <c r="E6">
-        <v>306.15</v>
+        <v>306.14999999999998</v>
       </c>
       <c r="F6">
         <v>293.39</v>
       </c>
       <c r="G6">
-        <v>283.79</v>
+        <v>283.79000000000002</v>
       </c>
       <c r="H6">
         <v>317.27</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7">
-        <v>37.48</v>
+        <v>37.479999999999997</v>
       </c>
       <c r="C7">
         <v>46.96</v>
@@ -692,7 +1018,7 @@
         <v>44.89</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -718,7 +1044,7 @@
         <v>10.77</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -732,7 +1058,7 @@
         <v>8</v>
       </c>
       <c r="E9">
-        <v>18.01</v>
+        <v>18.010000000000002</v>
       </c>
       <c r="F9">
         <v>19.84</v>
@@ -744,7 +1070,7 @@
         <v>9.58</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -767,10 +1093,10 @@
         <v>7.44</v>
       </c>
       <c r="H10">
-        <v>8.380000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>8.3800000000000008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -793,15 +1119,15 @@
         <v>96</v>
       </c>
       <c r="H11">
-        <v>97.34999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>97.35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B12">
-        <v>70.45999999999999</v>
+        <v>70.459999999999994</v>
       </c>
       <c r="C12">
         <v>70.31</v>
@@ -810,7 +1136,7 @@
         <v>58.8</v>
       </c>
       <c r="E12">
-        <v>72.43000000000001</v>
+        <v>72.430000000000007</v>
       </c>
       <c r="F12">
         <v>79.27</v>
@@ -822,7 +1148,7 @@
         <v>55.18</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -848,7 +1174,7 @@
         <v>14.96</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -874,7 +1200,7 @@
         <v>428.27</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -900,7 +1226,7 @@
         <v>8.85</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -926,7 +1252,7 @@
         <v>65.63</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -952,7 +1278,7 @@
         <v>33.4</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -966,7 +1292,7 @@
         <v>20.29</v>
       </c>
       <c r="E18">
-        <v>20.42</v>
+        <v>20.420000000000002</v>
       </c>
       <c r="F18">
         <v>20.16</v>
@@ -978,7 +1304,7 @@
         <v>25.59</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -995,16 +1321,16 @@
         <v>68.08</v>
       </c>
       <c r="F19">
-        <v>66.59999999999999</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="G19">
-        <v>70.93000000000001</v>
+        <v>70.930000000000007</v>
       </c>
       <c r="H19">
         <v>88.02</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1018,7 +1344,7 @@
         <v>6.69</v>
       </c>
       <c r="E20">
-        <v>8.050000000000001</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F20">
         <v>7.49</v>
@@ -1030,24 +1356,24 @@
         <v>8.69</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B21">
-        <v>19.51</v>
+        <v>19.510000000000002</v>
       </c>
       <c r="C21">
         <v>16.29</v>
       </c>
       <c r="D21">
-        <v>16.01</v>
+        <v>16.010000000000002</v>
       </c>
       <c r="E21">
         <v>10.63</v>
       </c>
       <c r="F21">
-        <v>9.630000000000001</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="G21">
         <v>16.68</v>
@@ -1056,12 +1382,12 @@
         <v>16.79</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B22">
-        <v>85.68000000000001</v>
+        <v>85.68</v>
       </c>
       <c r="C22">
         <v>107.15</v>
@@ -1076,13 +1402,13 @@
         <v>144.65</v>
       </c>
       <c r="G22">
-        <v>841.8200000000001</v>
+        <v>841.82</v>
       </c>
       <c r="H22">
         <v>375.34</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -1102,13 +1428,13 @@
         <v>425.97</v>
       </c>
       <c r="G23">
-        <v>671.4400000000001</v>
+        <v>671.44</v>
       </c>
       <c r="H23">
         <v>466.58</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1125,7 +1451,7 @@
         <v>2469</v>
       </c>
       <c r="F24">
-        <v>2124.43</v>
+        <v>2124.4299999999998</v>
       </c>
       <c r="G24">
         <v>1981.78</v>
@@ -1134,7 +1460,7 @@
         <v>1787.97</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1151,7 +1477,7 @@
         <v>659.51</v>
       </c>
       <c r="F25">
-        <v>599.0599999999999</v>
+        <v>599.05999999999995</v>
       </c>
       <c r="G25">
         <v>562.14</v>
@@ -1160,15 +1486,15 @@
         <v>545.72</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B26">
-        <v>86.31999999999999</v>
+        <v>86.32</v>
       </c>
       <c r="C26">
-        <v>99.15000000000001</v>
+        <v>99.15</v>
       </c>
       <c r="D26">
         <v>126.56</v>
@@ -1180,13 +1506,13 @@
         <v>109.24</v>
       </c>
       <c r="G26">
-        <v>73.56999999999999</v>
+        <v>73.569999999999993</v>
       </c>
       <c r="H26">
         <v>81.13</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -1209,15 +1535,15 @@
         <v>8.07</v>
       </c>
       <c r="H27">
-        <v>8.380000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>8.3800000000000008</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B28">
-        <v>9.050000000000001</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="C28">
         <v>22.32</v>
@@ -1238,7 +1564,7 @@
         <v>3.91</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -1246,7 +1572,7 @@
         <v>841.17</v>
       </c>
       <c r="C29">
-        <v>891.1799999999999</v>
+        <v>891.18</v>
       </c>
       <c r="D29">
         <v>922.41</v>
@@ -1264,7 +1590,7 @@
         <v>810.09</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1290,7 +1616,7 @@
         <v>29.32</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -1298,7 +1624,7 @@
         <v>2197.31</v>
       </c>
       <c r="C31">
-        <v>2171.97</v>
+        <v>2171.9699999999998</v>
       </c>
       <c r="D31">
         <v>1736.42</v>
@@ -1317,154 +1643,114 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B15">
-    <cfRule type="notContainsErrors" dxfId="0" priority="14">
+  <conditionalFormatting sqref="B15:B19">
+    <cfRule type="notContainsErrors" dxfId="43" priority="14">
       <formula>NOT(ISERROR(B15))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="notContainsErrors" dxfId="0" priority="15">
-      <formula>NOT(ISERROR(B16))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="notContainsErrors" dxfId="0" priority="16">
-      <formula>NOT(ISERROR(B17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="notContainsErrors" dxfId="0" priority="17">
-      <formula>NOT(ISERROR(B18))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="notContainsErrors" dxfId="0" priority="18">
-      <formula>NOT(ISERROR(B19))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22">
-    <cfRule type="notContainsErrors" dxfId="0" priority="21">
+  <conditionalFormatting sqref="B22:B23">
+    <cfRule type="notContainsErrors" dxfId="42" priority="21">
       <formula>NOT(ISERROR(B22))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
-    <cfRule type="notContainsErrors" dxfId="0" priority="22">
-      <formula>NOT(ISERROR(B23))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="notContainsErrors" dxfId="0" priority="4">
+    <cfRule type="notContainsErrors" dxfId="41" priority="4">
       <formula>NOT(ISERROR(C5))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D7:D8">
+    <cfRule type="notContainsErrors" dxfId="40" priority="6">
+      <formula>NOT(ISERROR(D7))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="notContainsErrors" dxfId="0" priority="9">
+    <cfRule type="notContainsErrors" dxfId="39" priority="9">
       <formula>NOT(ISERROR(D10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="notContainsErrors" dxfId="0" priority="12">
+    <cfRule type="notContainsErrors" dxfId="38" priority="12">
       <formula>NOT(ISERROR(D13))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="notContainsErrors" dxfId="0" priority="27">
+    <cfRule type="notContainsErrors" dxfId="37" priority="27">
       <formula>NOT(ISERROR(D28))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="notContainsErrors" dxfId="0" priority="6">
-      <formula>NOT(ISERROR(D7))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="notContainsErrors" dxfId="0" priority="7">
-      <formula>NOT(ISERROR(D8))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="notContainsErrors" dxfId="0" priority="10">
+    <cfRule type="notContainsErrors" dxfId="36" priority="10">
       <formula>NOT(ISERROR(E11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="notContainsErrors" dxfId="0" priority="29">
+    <cfRule type="notContainsErrors" dxfId="35" priority="29">
       <formula>NOT(ISERROR(E30))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="notContainsErrors" dxfId="0" priority="20">
+    <cfRule type="notContainsErrors" dxfId="34" priority="20">
       <formula>NOT(ISERROR(F21))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="notContainsErrors" dxfId="33" priority="2">
+      <formula>NOT(ISERROR(G3))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="notContainsErrors" dxfId="32" priority="5">
+      <formula>NOT(ISERROR(G6))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="notContainsErrors" dxfId="31" priority="8">
+      <formula>NOT(ISERROR(G9))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="notContainsErrors" dxfId="0" priority="13">
+    <cfRule type="notContainsErrors" dxfId="30" priority="13">
       <formula>NOT(ISERROR(G14))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="notContainsErrors" dxfId="0" priority="19">
+    <cfRule type="notContainsErrors" dxfId="29" priority="19">
       <formula>NOT(ISERROR(G20))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G26">
-    <cfRule type="notContainsErrors" dxfId="0" priority="25">
+  <conditionalFormatting sqref="G26:G27">
+    <cfRule type="notContainsErrors" dxfId="28" priority="25">
       <formula>NOT(ISERROR(G26))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G27">
-    <cfRule type="notContainsErrors" dxfId="0" priority="26">
-      <formula>NOT(ISERROR(G27))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="notContainsErrors" dxfId="0" priority="28">
+    <cfRule type="notContainsErrors" dxfId="27" priority="28">
       <formula>NOT(ISERROR(G29))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3">
-    <cfRule type="notContainsErrors" dxfId="0" priority="2">
-      <formula>NOT(ISERROR(G3))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G31">
-    <cfRule type="notContainsErrors" dxfId="0" priority="30">
+    <cfRule type="notContainsErrors" dxfId="26" priority="30">
       <formula>NOT(ISERROR(G31))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="notContainsErrors" dxfId="0" priority="5">
-      <formula>NOT(ISERROR(G6))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
-    <cfRule type="notContainsErrors" dxfId="0" priority="8">
-      <formula>NOT(ISERROR(G9))</formula>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="notContainsErrors" dxfId="25" priority="1">
+      <formula>NOT(ISERROR(H2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="notContainsErrors" dxfId="24" priority="3">
+      <formula>NOT(ISERROR(H4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="notContainsErrors" dxfId="0" priority="11">
+    <cfRule type="notContainsErrors" dxfId="23" priority="11">
       <formula>NOT(ISERROR(H12))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
-    <cfRule type="notContainsErrors" dxfId="0" priority="1">
-      <formula>NOT(ISERROR(H2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
-    <cfRule type="notContainsErrors" dxfId="0" priority="23">
+  <conditionalFormatting sqref="H24:H25">
+    <cfRule type="notContainsErrors" dxfId="22" priority="23">
       <formula>NOT(ISERROR(H24))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25">
-    <cfRule type="notContainsErrors" dxfId="0" priority="24">
-      <formula>NOT(ISERROR(H25))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="notContainsErrors" dxfId="0" priority="3">
-      <formula>NOT(ISERROR(H4))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1472,14 +1758,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1505,7 +1800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1519,7 +1814,7 @@
         <v>907298</v>
       </c>
       <c r="E2">
-        <v>913766.4</v>
+        <v>913766.40000000002</v>
       </c>
       <c r="F2">
         <v>913178</v>
@@ -1531,7 +1826,7 @@
         <v>906408</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1545,7 +1840,7 @@
         <v>906885.6</v>
       </c>
       <c r="E3">
-        <v>913766.4</v>
+        <v>913766.40000000002</v>
       </c>
       <c r="F3">
         <v>913178</v>
@@ -1557,7 +1852,7 @@
         <v>907149.2</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1565,7 +1860,7 @@
         <v>480774.8</v>
       </c>
       <c r="C4">
-        <v>480678.4</v>
+        <v>480678.40000000002</v>
       </c>
       <c r="D4">
         <v>484748</v>
@@ -1577,13 +1872,13 @@
         <v>486655.6</v>
       </c>
       <c r="G4">
-        <v>481612.8</v>
+        <v>481612.79999999999</v>
       </c>
       <c r="H4">
         <v>485016.8</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1591,7 +1886,7 @@
         <v>54014.8</v>
       </c>
       <c r="C5">
-        <v>53427.2</v>
+        <v>53427.199999999997</v>
       </c>
       <c r="D5">
         <v>54658</v>
@@ -1609,7 +1904,7 @@
         <v>53802</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1635,7 +1930,7 @@
         <v>190004.8</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1661,7 +1956,7 @@
         <v>11348.4</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1672,7 +1967,7 @@
         <v>2444</v>
       </c>
       <c r="D8">
-        <v>2415.2</v>
+        <v>2415.1999999999998</v>
       </c>
       <c r="E8">
         <v>2564.4</v>
@@ -1684,10 +1979,10 @@
         <v>2476.4</v>
       </c>
       <c r="H8">
-        <v>2428.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>2428.8000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1713,7 +2008,7 @@
         <v>1725.6</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1721,7 +2016,7 @@
         <v>5158.8</v>
       </c>
       <c r="C10">
-        <v>5153.6</v>
+        <v>5153.6000000000004</v>
       </c>
       <c r="D10">
         <v>5229.2</v>
@@ -1739,7 +2034,7 @@
         <v>5128</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1750,7 +2045,7 @@
         <v>75232</v>
       </c>
       <c r="D11">
-        <v>75116.8</v>
+        <v>75116.800000000003</v>
       </c>
       <c r="E11">
         <v>74978</v>
@@ -1759,13 +2054,13 @@
         <v>135647.6</v>
       </c>
       <c r="G11">
-        <v>75107.2</v>
+        <v>75107.199999999997</v>
       </c>
       <c r="H11">
         <v>74960</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1779,7 +2074,7 @@
         <v>16254</v>
       </c>
       <c r="E12">
-        <v>17180.4</v>
+        <v>17180.400000000001</v>
       </c>
       <c r="F12">
         <v>18382.8</v>
@@ -1791,7 +2086,7 @@
         <v>16245.6</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1817,18 +2112,18 @@
         <v>11210.4</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B14">
-        <v>330089.6</v>
+        <v>330089.59999999998</v>
       </c>
       <c r="C14">
         <v>330817.2</v>
       </c>
       <c r="D14">
-        <v>330659.2</v>
+        <v>330659.20000000001</v>
       </c>
       <c r="E14">
         <v>330465.2</v>
@@ -1837,13 +2132,13 @@
         <v>331183.2</v>
       </c>
       <c r="G14">
-        <v>330901.6</v>
+        <v>330901.59999999998</v>
       </c>
       <c r="H14">
-        <v>330639.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>330639.59999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1869,41 +2164,41 @@
         <v>7780.4</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B16">
-        <v>60305.6</v>
+        <v>60305.599999999999</v>
       </c>
       <c r="C16">
-        <v>60138.4</v>
+        <v>60138.400000000001</v>
       </c>
       <c r="D16">
-        <v>60276.8</v>
+        <v>60276.800000000003</v>
       </c>
       <c r="E16">
         <v>60074.8</v>
       </c>
       <c r="F16">
-        <v>60216.8</v>
+        <v>60216.800000000003</v>
       </c>
       <c r="G16">
-        <v>60180.8</v>
+        <v>60180.800000000003</v>
       </c>
       <c r="H16">
         <v>60090.8</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B17">
-        <v>31831.6</v>
+        <v>31831.599999999999</v>
       </c>
       <c r="C17">
-        <v>31823.6</v>
+        <v>31823.599999999999</v>
       </c>
       <c r="D17">
         <v>31788</v>
@@ -1912,30 +2207,30 @@
         <v>31746</v>
       </c>
       <c r="F17">
-        <v>31747.2</v>
+        <v>31747.200000000001</v>
       </c>
       <c r="G17">
-        <v>31760.8</v>
+        <v>31760.799999999999</v>
       </c>
       <c r="H17">
-        <v>31843.6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>31843.599999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B18">
-        <v>21544.8</v>
+        <v>21544.799999999999</v>
       </c>
       <c r="C18">
         <v>21432</v>
       </c>
       <c r="D18">
-        <v>21528.8</v>
+        <v>21528.799999999999</v>
       </c>
       <c r="E18">
-        <v>21510.4</v>
+        <v>21510.400000000001</v>
       </c>
       <c r="F18">
         <v>21452</v>
@@ -1944,24 +2239,24 @@
         <v>21476</v>
       </c>
       <c r="H18">
-        <v>21529.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>21529.599999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B19">
-        <v>77113.60000000001</v>
+        <v>77113.600000000006</v>
       </c>
       <c r="C19">
-        <v>78060.8</v>
+        <v>78060.800000000003</v>
       </c>
       <c r="D19">
-        <v>78573.60000000001</v>
+        <v>78573.600000000006</v>
       </c>
       <c r="E19">
-        <v>77691.2</v>
+        <v>77691.199999999997</v>
       </c>
       <c r="F19">
         <v>77477.2</v>
@@ -1973,7 +2268,7 @@
         <v>78454</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1987,10 +2282,10 @@
         <v>3915.2</v>
       </c>
       <c r="E20">
-        <v>4423.6</v>
+        <v>4423.6000000000004</v>
       </c>
       <c r="F20">
-        <v>4260.4</v>
+        <v>4260.3999999999996</v>
       </c>
       <c r="G20">
         <v>3776.8</v>
@@ -1999,7 +2294,7 @@
         <v>3620.4</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -2010,13 +2305,13 @@
         <v>3551.2</v>
       </c>
       <c r="D21">
-        <v>4586.4</v>
+        <v>4586.3999999999996</v>
       </c>
       <c r="E21">
         <v>2278</v>
       </c>
       <c r="F21">
-        <v>2063.2</v>
+        <v>2063.1999999999998</v>
       </c>
       <c r="G21">
         <v>4732</v>
@@ -2025,7 +2320,7 @@
         <v>3798.4</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -2051,7 +2346,7 @@
         <v>1321.2</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -2077,7 +2372,7 @@
         <v>409662.4</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -2103,7 +2398,7 @@
         <v>905704.4</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -2117,7 +2412,7 @@
         <v>249782.8</v>
       </c>
       <c r="E25">
-        <v>275144.4</v>
+        <v>275144.40000000002</v>
       </c>
       <c r="F25">
         <v>270699.2</v>
@@ -2129,33 +2424,33 @@
         <v>257969.2</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B26">
-        <v>36418.4</v>
+        <v>36418.400000000001</v>
       </c>
       <c r="C26">
-        <v>43484.8</v>
+        <v>43484.800000000003</v>
       </c>
       <c r="D26">
-        <v>37610.4</v>
+        <v>37610.400000000001</v>
       </c>
       <c r="E26">
-        <v>54497.6</v>
+        <v>54497.599999999999</v>
       </c>
       <c r="F26">
         <v>46721.2</v>
       </c>
       <c r="G26">
-        <v>35418.8</v>
+        <v>35418.800000000003</v>
       </c>
       <c r="H26">
-        <v>36631.6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>36631.599999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -2163,7 +2458,7 @@
         <v>3175.6</v>
       </c>
       <c r="C27">
-        <v>4787.6</v>
+        <v>4787.6000000000004</v>
       </c>
       <c r="D27">
         <v>3236.8</v>
@@ -2181,7 +2476,7 @@
         <v>3191.6</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -2204,10 +2499,10 @@
         <v>2689.2</v>
       </c>
       <c r="H28">
-        <v>294.4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>294.39999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -2233,7 +2528,7 @@
         <v>386534.8</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -2244,13 +2539,13 @@
         <v>18574.8</v>
       </c>
       <c r="D30">
-        <v>17920.4</v>
+        <v>17920.400000000001</v>
       </c>
       <c r="E30">
         <v>18583.2</v>
       </c>
       <c r="F30">
-        <v>18478.4</v>
+        <v>18478.400000000001</v>
       </c>
       <c r="G30">
         <v>17906</v>
@@ -2259,7 +2554,7 @@
         <v>18046.8</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -2286,148 +2581,108 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="notContainsErrors" dxfId="21" priority="6">
+      <formula>NOT(ISERROR(B7))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="notContainsErrors" dxfId="0" priority="11">
+    <cfRule type="notContainsErrors" dxfId="20" priority="11">
       <formula>NOT(ISERROR(B12))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="notContainsErrors" dxfId="0" priority="13">
+  <conditionalFormatting sqref="B14:B15">
+    <cfRule type="notContainsErrors" dxfId="19" priority="13">
       <formula>NOT(ISERROR(B14))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
-    <cfRule type="notContainsErrors" dxfId="0" priority="14">
-      <formula>NOT(ISERROR(B15))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="notContainsErrors" dxfId="0" priority="18">
+    <cfRule type="notContainsErrors" dxfId="18" priority="18">
       <formula>NOT(ISERROR(B19))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="notContainsErrors" dxfId="0" priority="26">
+    <cfRule type="notContainsErrors" dxfId="17" priority="26">
       <formula>NOT(ISERROR(B27))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="notContainsErrors" dxfId="0" priority="29">
+    <cfRule type="notContainsErrors" dxfId="16" priority="29">
       <formula>NOT(ISERROR(B30))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="notContainsErrors" dxfId="0" priority="6">
-      <formula>NOT(ISERROR(B7))</formula>
+  <conditionalFormatting sqref="C2:C6">
+    <cfRule type="notContainsErrors" dxfId="15" priority="1">
+      <formula>NOT(ISERROR(C2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="notContainsErrors" dxfId="0" priority="12">
+    <cfRule type="notContainsErrors" dxfId="14" priority="12">
       <formula>NOT(ISERROR(C13))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="notContainsErrors" dxfId="0" priority="17">
+    <cfRule type="notContainsErrors" dxfId="13" priority="17">
       <formula>NOT(ISERROR(C18))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="notContainsErrors" dxfId="0" priority="1">
-      <formula>NOT(ISERROR(C2))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="notContainsErrors" dxfId="0" priority="21">
+    <cfRule type="notContainsErrors" dxfId="12" priority="21">
       <formula>NOT(ISERROR(C22))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="notContainsErrors" dxfId="0" priority="2">
-      <formula>NOT(ISERROR(C3))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4">
-    <cfRule type="notContainsErrors" dxfId="0" priority="3">
-      <formula>NOT(ISERROR(C4))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5">
-    <cfRule type="notContainsErrors" dxfId="0" priority="4">
-      <formula>NOT(ISERROR(C5))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6">
-    <cfRule type="notContainsErrors" dxfId="0" priority="5">
-      <formula>NOT(ISERROR(C6))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
-    <cfRule type="notContainsErrors" dxfId="0" priority="23">
+  <conditionalFormatting sqref="D8">
+    <cfRule type="notContainsErrors" dxfId="11" priority="7">
+      <formula>NOT(ISERROR(D8))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24:D25">
+    <cfRule type="notContainsErrors" dxfId="10" priority="23">
       <formula>NOT(ISERROR(D24))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="notContainsErrors" dxfId="0" priority="24">
-      <formula>NOT(ISERROR(D25))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="notContainsErrors" dxfId="0" priority="7">
-      <formula>NOT(ISERROR(D8))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
-    <cfRule type="notContainsErrors" dxfId="0" priority="15">
+  <conditionalFormatting sqref="E16:E17">
+    <cfRule type="notContainsErrors" dxfId="9" priority="15">
       <formula>NOT(ISERROR(E16))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="notContainsErrors" dxfId="0" priority="16">
-      <formula>NOT(ISERROR(E17))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="notContainsErrors" dxfId="0" priority="27">
+    <cfRule type="notContainsErrors" dxfId="8" priority="27">
       <formula>NOT(ISERROR(E28))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="notContainsErrors" dxfId="0" priority="20">
+    <cfRule type="notContainsErrors" dxfId="7" priority="20">
       <formula>NOT(ISERROR(F21))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31">
-    <cfRule type="notContainsErrors" dxfId="0" priority="30">
+    <cfRule type="notContainsErrors" dxfId="6" priority="30">
       <formula>NOT(ISERROR(F31))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="notContainsErrors" dxfId="5" priority="8">
+      <formula>NOT(ISERROR(G9))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="notContainsErrors" dxfId="0" priority="25">
+    <cfRule type="notContainsErrors" dxfId="4" priority="25">
       <formula>NOT(ISERROR(G26))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
-    <cfRule type="notContainsErrors" dxfId="0" priority="8">
-      <formula>NOT(ISERROR(G9))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="notContainsErrors" dxfId="0" priority="9">
+  <conditionalFormatting sqref="H10:H11">
+    <cfRule type="notContainsErrors" dxfId="3" priority="9">
       <formula>NOT(ISERROR(H10))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
-    <cfRule type="notContainsErrors" dxfId="0" priority="10">
-      <formula>NOT(ISERROR(H11))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="notContainsErrors" dxfId="0" priority="19">
+    <cfRule type="notContainsErrors" dxfId="2" priority="19">
       <formula>NOT(ISERROR(H20))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="notContainsErrors" dxfId="0" priority="22">
+    <cfRule type="notContainsErrors" dxfId="1" priority="22">
       <formula>NOT(ISERROR(H23))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>